<commit_message>
Correct metadata and use separate file from @wilsonsj100
</commit_message>
<xml_diff>
--- a/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
+++ b/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Biogeochemistry\People\Wilson (Steph)\Data\Fluxes\Chamber Fluxes\Data for Ben\All_2022_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B2A871-CFF2-4999-B73B-17B4DECD293C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9775C0C-90B4-4380-95E2-878CFBABCDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
+    <workbookView xWindow="90" yWindow="45" windowWidth="16155" windowHeight="11340" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPASS_ChamberFlux_Metadata_20" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -423,6 +423,15 @@
   </si>
   <si>
     <t>Repeat bc first one had bad CO2 slope</t>
+  </si>
+  <si>
+    <t>w/o increase</t>
+  </si>
+  <si>
+    <t>used 8 clips on top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">different grass spp than other 4 </t>
   </si>
 </sst>
 </file>
@@ -500,12 +509,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -820,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5B7D07-181D-BE46-BEC5-DBDE824ED711}">
-  <dimension ref="A1:L119"/>
+  <dimension ref="A1:L120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1616,10 +1628,10 @@
         <v>44756</v>
       </c>
       <c r="B21" s="3">
-        <v>0.62361111111111112</v>
+        <v>0.31805555555555554</v>
       </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D21">
         <v>0.16</v>
@@ -1628,7 +1640,6 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <f>E21*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G21" t="s">
@@ -1647,7 +1658,7 @@
         <v>30</v>
       </c>
       <c r="L21" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -1655,10 +1666,10 @@
         <v>44756</v>
       </c>
       <c r="B22" s="3">
-        <v>0.62951388888888882</v>
+        <v>0.32361111111111113</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D22">
         <v>0.16</v>
@@ -1667,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" ref="F22:F39" si="1">E22*0.064</f>
+        <f>E22*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G22" t="s">
@@ -1680,7 +1691,7 @@
         <v>32</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K22">
         <v>30</v>
@@ -1694,10 +1705,10 @@
         <v>44756</v>
       </c>
       <c r="B23" s="3">
-        <v>0.63472222222222219</v>
+        <v>0.32916666666666666</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>0.16</v>
@@ -1706,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F23:F40" si="1">E23*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G23" t="s">
@@ -1719,7 +1730,7 @@
         <v>32</v>
       </c>
       <c r="J23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23">
         <v>30</v>
@@ -1733,10 +1744,10 @@
         <v>44756</v>
       </c>
       <c r="B24" s="3">
-        <v>0.64236111111111105</v>
+        <v>0.33611111111111108</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24">
         <v>0.16</v>
@@ -1758,7 +1769,7 @@
         <v>32</v>
       </c>
       <c r="J24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K24">
         <v>30</v>
@@ -1769,41 +1780,41 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>44754</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0.3972222222222222</v>
+        <v>44756</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.34097222222222223</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>0.16</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F25">
         <f t="shared" si="1"/>
-        <v>0.25600000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="G25" t="s">
         <v>7</v>
       </c>
       <c r="H25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K25">
-        <v>29.444400000000002</v>
+        <v>30</v>
       </c>
       <c r="L25" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1811,20 +1822,20 @@
         <v>44754</v>
       </c>
       <c r="B26" s="3">
-        <v>0.4375</v>
+        <v>0.44513888888888892</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D26">
         <v>0.16</v>
       </c>
       <c r="E26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F26">
         <f t="shared" si="1"/>
-        <v>0.25600000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="G26" t="s">
         <v>7</v>
@@ -1836,7 +1847,7 @@
         <v>34</v>
       </c>
       <c r="J26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K26">
         <v>29.444400000000002</v>
@@ -1850,10 +1861,10 @@
         <v>44754</v>
       </c>
       <c r="B27" s="3">
-        <v>0.41215277777777781</v>
+        <v>0.46388888888888885</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27">
         <v>0.16</v>
@@ -1875,7 +1886,7 @@
         <v>34</v>
       </c>
       <c r="J27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K27">
         <v>29.444400000000002</v>
@@ -1889,10 +1900,10 @@
         <v>44754</v>
       </c>
       <c r="B28" s="3">
-        <v>0.4236111111111111</v>
+        <v>0.47291666666666665</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D28">
         <v>0.16</v>
@@ -1914,7 +1925,7 @@
         <v>34</v>
       </c>
       <c r="J28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K28">
         <v>29.444400000000002</v>
@@ -1928,20 +1939,20 @@
         <v>44754</v>
       </c>
       <c r="B29" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.48055555555555557</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D29">
         <v>0.16</v>
       </c>
       <c r="E29">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F29">
         <f t="shared" si="1"/>
-        <v>0.25600000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="G29" t="s">
         <v>7</v>
@@ -1953,7 +1964,7 @@
         <v>34</v>
       </c>
       <c r="J29">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K29">
         <v>29.444400000000002</v>
@@ -1967,20 +1978,20 @@
         <v>44754</v>
       </c>
       <c r="B30" s="3">
-        <v>0.34236111111111112</v>
+        <v>0.4909722222222222</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30">
         <v>0.16</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30">
         <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.192</v>
       </c>
       <c r="G30" t="s">
         <v>7</v>
@@ -1989,10 +2000,10 @@
         <v>33</v>
       </c>
       <c r="I30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K30">
         <v>29.444400000000002</v>
@@ -2006,20 +2017,20 @@
         <v>44754</v>
       </c>
       <c r="B31" s="3">
-        <v>0.34722222222222227</v>
+        <v>0.39641203703703703</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>0.16</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F31">
         <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G31" t="s">
         <v>7</v>
@@ -2031,7 +2042,7 @@
         <v>32</v>
       </c>
       <c r="J31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <v>29.444400000000002</v>
@@ -2045,20 +2056,20 @@
         <v>44754</v>
       </c>
       <c r="B32" s="3">
-        <v>0.3520833333333333</v>
+        <v>0.40162037037037041</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32">
         <v>0.16</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G32" t="s">
         <v>7</v>
@@ -2070,7 +2081,7 @@
         <v>32</v>
       </c>
       <c r="J32">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K32">
         <v>29.444400000000002</v>
@@ -2084,20 +2095,20 @@
         <v>44754</v>
       </c>
       <c r="B33" s="3">
-        <v>0.35833333333333334</v>
+        <v>0.40833333333333338</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D33">
         <v>0.16</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G33" t="s">
         <v>7</v>
@@ -2109,7 +2120,7 @@
         <v>32</v>
       </c>
       <c r="J33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K33">
         <v>29.444400000000002</v>
@@ -2123,20 +2134,20 @@
         <v>44754</v>
       </c>
       <c r="B34" s="3">
-        <v>0.36388888888888887</v>
+        <v>0.4152777777777778</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34">
         <v>0.16</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <f t="shared" si="1"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G34" t="s">
         <v>7</v>
@@ -2148,7 +2159,7 @@
         <v>32</v>
       </c>
       <c r="J34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K34">
         <v>29.444400000000002</v>
@@ -2159,13 +2170,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>44753</v>
+        <v>44754</v>
       </c>
       <c r="B35" s="3">
-        <v>0.56770833333333337</v>
+        <v>0.42152777777777778</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35">
         <v>0.16</v>
@@ -2181,213 +2192,213 @@
         <v>7</v>
       </c>
       <c r="H35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I35" t="s">
         <v>32</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K35">
-        <v>30</v>
+        <v>29.444400000000002</v>
       </c>
       <c r="L35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
         <v>44753</v>
       </c>
-      <c r="B36" s="3">
-        <v>0.57986111111111105</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36">
-        <v>0.16</v>
-      </c>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
+      <c r="B36" s="6">
+        <v>0.3840277777777778</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E36" s="7">
+        <v>2</v>
+      </c>
+      <c r="F36" s="7">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G36" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="G36" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I36" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36">
-        <v>2</v>
-      </c>
-      <c r="K36">
+      <c r="I36" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="7">
+        <v>1</v>
+      </c>
+      <c r="K36" s="7">
         <v>30</v>
       </c>
-      <c r="L36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="L36" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>44753</v>
       </c>
-      <c r="B37" s="3">
-        <v>0.59652777777777777</v>
-      </c>
-      <c r="C37" t="s">
-        <v>25</v>
-      </c>
-      <c r="D37">
-        <v>0.16</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
+      <c r="B37" s="6">
+        <v>0.39444444444444443</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="7">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G37" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="G37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I37" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37">
-        <v>3</v>
-      </c>
-      <c r="K37">
+      <c r="I37" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" s="7">
+        <v>2</v>
+      </c>
+      <c r="K37" s="7">
         <v>30</v>
       </c>
-      <c r="L37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="L37" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>44753</v>
       </c>
-      <c r="B38" s="3">
-        <v>0.59166666666666667</v>
-      </c>
-      <c r="C38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38">
-        <v>0.16</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38">
+      <c r="B38" s="6">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E38" s="7">
+        <v>2</v>
+      </c>
+      <c r="F38" s="7">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="G38" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I38" t="s">
-        <v>32</v>
-      </c>
-      <c r="J38">
-        <v>4</v>
-      </c>
-      <c r="K38">
+      <c r="I38" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" s="7">
+        <v>3</v>
+      </c>
+      <c r="K38" s="7">
         <v>30</v>
       </c>
-      <c r="L38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="L38" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
         <v>44753</v>
       </c>
-      <c r="B39" s="3">
-        <v>0.60277777777777775</v>
-      </c>
-      <c r="C39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39">
-        <v>0.16</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="F39">
+      <c r="B39" s="6">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E39" s="7">
+        <v>2</v>
+      </c>
+      <c r="F39" s="7">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G39" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="G39" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I39" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39">
+      <c r="I39" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" s="7">
+        <v>4</v>
+      </c>
+      <c r="K39" s="7">
+        <v>30</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>44753</v>
+      </c>
+      <c r="B40" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E40" s="7">
+        <v>2</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" si="1"/>
+        <v>0.128</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40" s="7">
         <v>5</v>
       </c>
-      <c r="K39">
+      <c r="K40" s="7">
         <v>30</v>
       </c>
-      <c r="L39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>44804</v>
-      </c>
-      <c r="B40" s="4">
-        <v>0.42766203703703703</v>
-      </c>
-      <c r="C40" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40">
-        <v>0.16</v>
-      </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
-        <f>E40*0.064</f>
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="G40" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" t="s">
-        <v>32</v>
-      </c>
-      <c r="J40">
-        <v>1</v>
-      </c>
-      <c r="K40">
-        <v>27.2</v>
-      </c>
-      <c r="L40" t="s">
+      <c r="L40" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2395,11 +2406,11 @@
       <c r="A41" s="1">
         <v>44804</v>
       </c>
-      <c r="B41" s="3">
-        <v>0.41782407407407413</v>
+      <c r="B41" s="4">
+        <v>0.42766203703703703</v>
       </c>
       <c r="C41" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D41">
         <v>0.16</v>
@@ -2421,7 +2432,7 @@
         <v>32</v>
       </c>
       <c r="J41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K41">
         <v>27.2</v>
@@ -2435,10 +2446,10 @@
         <v>44804</v>
       </c>
       <c r="B42" s="3">
-        <v>0.40856481481481483</v>
+        <v>0.41782407407407413</v>
       </c>
       <c r="C42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D42">
         <v>0.16</v>
@@ -2447,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <f t="shared" ref="F42:F59" si="2">E42*0.064</f>
+        <f>E42*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G42" t="s">
@@ -2460,7 +2471,7 @@
         <v>32</v>
       </c>
       <c r="J42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K42">
         <v>27.2</v>
@@ -2474,10 +2485,10 @@
         <v>44804</v>
       </c>
       <c r="B43" s="3">
-        <v>0.39988425925925924</v>
+        <v>0.40856481481481483</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D43">
         <v>0.16</v>
@@ -2486,7 +2497,7 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F43:F60" si="2">E43*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G43" t="s">
@@ -2499,7 +2510,7 @@
         <v>32</v>
       </c>
       <c r="J43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K43">
         <v>27.2</v>
@@ -2513,10 +2524,10 @@
         <v>44804</v>
       </c>
       <c r="B44" s="3">
-        <v>0.39178240740740744</v>
+        <v>0.39988425925925924</v>
       </c>
       <c r="C44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D44">
         <v>0.16</v>
@@ -2538,7 +2549,7 @@
         <v>32</v>
       </c>
       <c r="J44">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K44">
         <v>27.2</v>
@@ -2549,41 +2560,41 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>44791</v>
+        <v>44804</v>
       </c>
       <c r="B45" s="3">
-        <v>0.45208333333333334</v>
+        <v>0.39178240740740744</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D45">
         <v>0.16</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>0.25600000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G45" t="s">
         <v>7</v>
       </c>
       <c r="H45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K45">
-        <v>29.5</v>
+        <v>27.2</v>
       </c>
       <c r="L45" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2591,10 +2602,10 @@
         <v>44791</v>
       </c>
       <c r="B46" s="3">
-        <v>0.44513888888888892</v>
+        <v>0.45208333333333334</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D46">
         <v>0.16</v>
@@ -2616,13 +2627,13 @@
         <v>34</v>
       </c>
       <c r="J46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <v>29.5</v>
       </c>
       <c r="L46" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
@@ -2630,10 +2641,10 @@
         <v>44791</v>
       </c>
       <c r="B47" s="3">
-        <v>0.4375</v>
+        <v>0.44513888888888892</v>
       </c>
       <c r="C47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47">
         <v>0.16</v>
@@ -2655,7 +2666,7 @@
         <v>34</v>
       </c>
       <c r="J47">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K47">
         <v>29.5</v>
@@ -2669,10 +2680,10 @@
         <v>44791</v>
       </c>
       <c r="B48" s="3">
-        <v>0.42777777777777781</v>
+        <v>0.4375</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>0.16</v>
@@ -2694,7 +2705,7 @@
         <v>34</v>
       </c>
       <c r="J48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K48">
         <v>29.5</v>
@@ -2708,10 +2719,10 @@
         <v>44791</v>
       </c>
       <c r="B49" s="3">
-        <v>0.4604166666666667</v>
+        <v>0.42777777777777781</v>
       </c>
       <c r="C49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D49">
         <v>0.16</v>
@@ -2733,13 +2744,13 @@
         <v>34</v>
       </c>
       <c r="J49">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K49">
         <v>29.5</v>
       </c>
       <c r="L49" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2747,20 +2758,20 @@
         <v>44791</v>
       </c>
       <c r="B50" s="3">
-        <v>0.39652777777777781</v>
+        <v>0.4604166666666667</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50">
         <v>0.16</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="G50" t="s">
         <v>7</v>
@@ -2769,16 +2780,16 @@
         <v>33</v>
       </c>
       <c r="I50" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J50">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K50">
         <v>29.5</v>
       </c>
       <c r="L50" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2786,10 +2797,10 @@
         <v>44791</v>
       </c>
       <c r="B51" s="3">
-        <v>0.40138888888888885</v>
+        <v>0.39652777777777781</v>
       </c>
       <c r="C51" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D51">
         <v>0.16</v>
@@ -2811,13 +2822,13 @@
         <v>32</v>
       </c>
       <c r="J51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K51">
         <v>29.5</v>
       </c>
       <c r="L51" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2825,10 +2836,10 @@
         <v>44791</v>
       </c>
       <c r="B52" s="3">
-        <v>0.40625</v>
+        <v>0.40138888888888885</v>
       </c>
       <c r="C52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D52">
         <v>0.16</v>
@@ -2850,13 +2861,13 @@
         <v>32</v>
       </c>
       <c r="J52">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K52">
         <v>29.5</v>
       </c>
       <c r="L52" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -2864,10 +2875,10 @@
         <v>44791</v>
       </c>
       <c r="B53" s="3">
-        <v>0.39097222222222222</v>
+        <v>0.40625</v>
       </c>
       <c r="C53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D53">
         <v>0.16</v>
@@ -2889,7 +2900,7 @@
         <v>32</v>
       </c>
       <c r="J53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K53">
         <v>29.5</v>
@@ -2903,10 +2914,10 @@
         <v>44791</v>
       </c>
       <c r="B54" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.39097222222222222</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D54">
         <v>0.16</v>
@@ -2928,7 +2939,7 @@
         <v>32</v>
       </c>
       <c r="J54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K54">
         <v>29.5</v>
@@ -2939,41 +2950,41 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>44788</v>
+        <v>44791</v>
       </c>
       <c r="B55" s="3">
-        <v>0.375</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55">
         <v>0.16</v>
       </c>
       <c r="E55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F55">
         <f t="shared" si="2"/>
-        <v>0.128</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G55" t="s">
         <v>7</v>
       </c>
       <c r="H55" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I55" t="s">
         <v>32</v>
       </c>
       <c r="J55">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K55">
-        <v>28.8</v>
+        <v>29.5</v>
       </c>
       <c r="L55" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
@@ -2981,10 +2992,10 @@
         <v>44788</v>
       </c>
       <c r="B56" s="3">
-        <v>0.38611111111111113</v>
+        <v>0.375</v>
       </c>
       <c r="C56" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56">
         <v>0.16</v>
@@ -3006,7 +3017,7 @@
         <v>32</v>
       </c>
       <c r="J56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K56">
         <v>28.8</v>
@@ -3020,10 +3031,10 @@
         <v>44788</v>
       </c>
       <c r="B57" s="3">
-        <v>0.3979166666666667</v>
+        <v>0.38611111111111113</v>
       </c>
       <c r="C57" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D57">
         <v>0.16</v>
@@ -3045,13 +3056,13 @@
         <v>32</v>
       </c>
       <c r="J57">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K57">
         <v>28.8</v>
       </c>
       <c r="L57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
@@ -3059,10 +3070,10 @@
         <v>44788</v>
       </c>
       <c r="B58" s="3">
-        <v>0.41597222222222219</v>
+        <v>0.3979166666666667</v>
       </c>
       <c r="C58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D58">
         <v>0.16</v>
@@ -3084,13 +3095,13 @@
         <v>32</v>
       </c>
       <c r="J58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K58">
         <v>28.8</v>
       </c>
       <c r="L58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
@@ -3098,10 +3109,10 @@
         <v>44788</v>
       </c>
       <c r="B59" s="3">
-        <v>0.42430555555555555</v>
+        <v>0.41597222222222219</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D59">
         <v>0.16</v>
@@ -3123,52 +3134,52 @@
         <v>32</v>
       </c>
       <c r="J59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K59">
         <v>28.8</v>
       </c>
       <c r="L59" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>44822</v>
+        <v>44788</v>
       </c>
       <c r="B60" s="3">
-        <v>0.31458333333333333</v>
+        <v>0.42430555555555555</v>
       </c>
       <c r="C60" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D60">
         <v>0.16</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F60">
-        <f t="shared" ref="F60:F81" si="3">E60*0.064</f>
-        <v>6.4000000000000001E-2</v>
+        <f t="shared" si="2"/>
+        <v>0.128</v>
       </c>
       <c r="G60" t="s">
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I60" t="s">
         <v>32</v>
       </c>
       <c r="J60">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K60">
-        <v>20.100000000000001</v>
+        <v>28.8</v>
       </c>
       <c r="L60" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
@@ -3176,10 +3187,10 @@
         <v>44822</v>
       </c>
       <c r="B61" s="3">
-        <v>0.31944444444444448</v>
+        <v>0.31458333333333333</v>
       </c>
       <c r="C61" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D61">
         <v>0.16</v>
@@ -3188,7 +3199,7 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F61:F82" si="3">E61*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G61" t="s">
@@ -3201,7 +3212,7 @@
         <v>32</v>
       </c>
       <c r="J61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <v>20.100000000000001</v>
@@ -3215,10 +3226,10 @@
         <v>44822</v>
       </c>
       <c r="B62" s="3">
-        <v>0.32430555555555557</v>
+        <v>0.31944444444444448</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D62">
         <v>0.16</v>
@@ -3240,7 +3251,7 @@
         <v>32</v>
       </c>
       <c r="J62">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K62">
         <v>20.100000000000001</v>
@@ -3254,10 +3265,10 @@
         <v>44822</v>
       </c>
       <c r="B63" s="3">
-        <v>0.3298611111111111</v>
+        <v>0.32430555555555557</v>
       </c>
       <c r="C63" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D63">
         <v>0.16</v>
@@ -3279,7 +3290,7 @@
         <v>32</v>
       </c>
       <c r="J63">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K63">
         <v>20.100000000000001</v>
@@ -3293,10 +3304,10 @@
         <v>44822</v>
       </c>
       <c r="B64" s="3">
-        <v>0.3354166666666667</v>
+        <v>0.3298611111111111</v>
       </c>
       <c r="C64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D64">
         <v>0.16</v>
@@ -3318,7 +3329,7 @@
         <v>32</v>
       </c>
       <c r="J64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K64">
         <v>20.100000000000001</v>
@@ -3329,41 +3340,41 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>44826</v>
+        <v>44822</v>
       </c>
       <c r="B65" s="3">
-        <v>0.42708333333333331</v>
+        <v>0.3354166666666667</v>
       </c>
       <c r="C65" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>0.16</v>
       </c>
       <c r="E65">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F65">
         <f t="shared" si="3"/>
-        <v>0.25600000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G65" t="s">
         <v>7</v>
       </c>
       <c r="H65" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J65">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K65">
-        <v>28.332999999999998</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="L65" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3371,10 +3382,10 @@
         <v>44826</v>
       </c>
       <c r="B66" s="3">
-        <v>0.41944444444444445</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D66">
         <v>0.16</v>
@@ -3396,13 +3407,13 @@
         <v>34</v>
       </c>
       <c r="J66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K66">
         <v>28.332999999999998</v>
       </c>
       <c r="L66" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3410,10 +3421,10 @@
         <v>44826</v>
       </c>
       <c r="B67" s="3">
-        <v>0.41180555555555554</v>
+        <v>0.41944444444444445</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67">
         <v>0.16</v>
@@ -3435,13 +3446,13 @@
         <v>34</v>
       </c>
       <c r="J67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K67">
         <v>28.332999999999998</v>
       </c>
       <c r="L67" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3449,10 +3460,10 @@
         <v>44826</v>
       </c>
       <c r="B68" s="3">
-        <v>0.40277777777777773</v>
+        <v>0.41180555555555554</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D68">
         <v>0.16</v>
@@ -3474,13 +3485,13 @@
         <v>34</v>
       </c>
       <c r="J68">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K68">
         <v>28.332999999999998</v>
       </c>
       <c r="L68" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
@@ -3488,10 +3499,10 @@
         <v>44826</v>
       </c>
       <c r="B69" s="3">
-        <v>0.43611111111111112</v>
+        <v>0.40277777777777773</v>
       </c>
       <c r="C69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D69">
         <v>0.16</v>
@@ -3513,13 +3524,13 @@
         <v>34</v>
       </c>
       <c r="J69">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K69">
         <v>28.332999999999998</v>
       </c>
       <c r="L69" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.25">
@@ -3527,20 +3538,20 @@
         <v>44826</v>
       </c>
       <c r="B70" s="3">
-        <v>0.38541666666666669</v>
+        <v>0.43611111111111112</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D70">
         <v>0.16</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F70">
         <f t="shared" si="3"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="G70" t="s">
         <v>7</v>
@@ -3549,13 +3560,13 @@
         <v>33</v>
       </c>
       <c r="I70" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J70">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K70">
-        <v>26.111000000000001</v>
+        <v>28.332999999999998</v>
       </c>
       <c r="L70" t="s">
         <v>39</v>
@@ -3566,10 +3577,10 @@
         <v>44826</v>
       </c>
       <c r="B71" s="3">
-        <v>0.38055555555555554</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="C71" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D71">
         <v>0.16</v>
@@ -3591,7 +3602,7 @@
         <v>32</v>
       </c>
       <c r="J71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K71">
         <v>26.111000000000001</v>
@@ -3605,10 +3616,10 @@
         <v>44826</v>
       </c>
       <c r="B72" s="3">
-        <v>0.37638888888888888</v>
+        <v>0.38055555555555554</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D72">
         <v>0.16</v>
@@ -3630,7 +3641,7 @@
         <v>32</v>
       </c>
       <c r="J72">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K72">
         <v>26.111000000000001</v>
@@ -3644,10 +3655,10 @@
         <v>44826</v>
       </c>
       <c r="B73" s="3">
-        <v>0.37187500000000001</v>
+        <v>0.37638888888888888</v>
       </c>
       <c r="C73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D73">
         <v>0.16</v>
@@ -3669,7 +3680,7 @@
         <v>32</v>
       </c>
       <c r="J73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K73">
         <v>26.111000000000001</v>
@@ -3683,10 +3694,10 @@
         <v>44826</v>
       </c>
       <c r="B74" s="3">
-        <v>0.36736111111111108</v>
+        <v>0.37187500000000001</v>
       </c>
       <c r="C74" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D74">
         <v>0.16</v>
@@ -3708,7 +3719,7 @@
         <v>32</v>
       </c>
       <c r="J74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K74">
         <v>26.111000000000001</v>
@@ -3719,41 +3730,41 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>44823</v>
+        <v>44826</v>
       </c>
       <c r="B75" s="3">
-        <v>0.39351851851851855</v>
+        <v>0.36736111111111108</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D75">
         <v>0.16</v>
       </c>
       <c r="E75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75">
         <f t="shared" si="3"/>
-        <v>0.128</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G75" t="s">
         <v>7</v>
       </c>
       <c r="H75" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I75" t="s">
         <v>32</v>
       </c>
       <c r="J75">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K75">
-        <v>28.332999999999998</v>
+        <v>26.111000000000001</v>
       </c>
       <c r="L75" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3761,10 +3772,10 @@
         <v>44823</v>
       </c>
       <c r="B76" s="3">
-        <v>0.40219907407407413</v>
+        <v>0.39351851851851855</v>
       </c>
       <c r="C76" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D76">
         <v>0.16</v>
@@ -3786,7 +3797,7 @@
         <v>32</v>
       </c>
       <c r="J76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K76">
         <v>28.332999999999998</v>
@@ -3800,10 +3811,10 @@
         <v>44823</v>
       </c>
       <c r="B77" s="3">
-        <v>0.41493055555555558</v>
+        <v>0.40219907407407413</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D77">
         <v>0.16</v>
@@ -3825,13 +3836,13 @@
         <v>32</v>
       </c>
       <c r="J77">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K77">
         <v>28.332999999999998</v>
       </c>
       <c r="L77" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.25">
@@ -3839,10 +3850,10 @@
         <v>44823</v>
       </c>
       <c r="B78" s="3">
-        <v>0.42476851851851855</v>
+        <v>0.41493055555555558</v>
       </c>
       <c r="C78" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D78">
         <v>0.16</v>
@@ -3864,13 +3875,13 @@
         <v>32</v>
       </c>
       <c r="J78">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K78">
         <v>28.332999999999998</v>
       </c>
       <c r="L78" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -3878,10 +3889,10 @@
         <v>44823</v>
       </c>
       <c r="B79" s="3">
-        <v>0.43888888888888888</v>
+        <v>0.42476851851851855</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D79">
         <v>0.16</v>
@@ -3903,52 +3914,52 @@
         <v>32</v>
       </c>
       <c r="J79">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K79">
         <v>28.332999999999998</v>
       </c>
       <c r="L79" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>44861</v>
+        <v>44823</v>
       </c>
       <c r="B80" s="3">
-        <v>0.35011574074074076</v>
+        <v>0.43888888888888888</v>
       </c>
       <c r="C80" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D80">
         <v>0.16</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F80">
         <f t="shared" si="3"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G80" t="s">
         <v>7</v>
       </c>
       <c r="H80" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I80" t="s">
         <v>32</v>
       </c>
       <c r="J80">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K80">
-        <v>15</v>
+        <v>28.332999999999998</v>
       </c>
       <c r="L80" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -3956,10 +3967,10 @@
         <v>44861</v>
       </c>
       <c r="B81" s="3">
-        <v>0.38483796296296297</v>
+        <v>0.35011574074074076</v>
       </c>
       <c r="C81" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D81">
         <v>0.16</v>
@@ -3981,7 +3992,7 @@
         <v>32</v>
       </c>
       <c r="J81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K81">
         <v>15</v>
@@ -3995,10 +4006,10 @@
         <v>44861</v>
       </c>
       <c r="B82" s="3">
-        <v>0.39756944444444442</v>
+        <v>0.38483796296296297</v>
       </c>
       <c r="C82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D82">
         <v>0.16</v>
@@ -4007,7 +4018,7 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <f t="shared" ref="F82:F103" si="4">E82*0.064</f>
+        <f t="shared" si="3"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G82" t="s">
@@ -4020,7 +4031,7 @@
         <v>32</v>
       </c>
       <c r="J82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K82">
         <v>15</v>
@@ -4034,10 +4045,10 @@
         <v>44861</v>
       </c>
       <c r="B83" s="3">
-        <v>0.37384259259259256</v>
+        <v>0.39756944444444442</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D83">
         <v>0.16</v>
@@ -4046,7 +4057,7 @@
         <v>1</v>
       </c>
       <c r="F83">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F83:F104" si="4">E83*0.064</f>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G83" t="s">
@@ -4059,7 +4070,7 @@
         <v>32</v>
       </c>
       <c r="J83">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K83">
         <v>15</v>
@@ -4073,10 +4084,10 @@
         <v>44861</v>
       </c>
       <c r="B84" s="3">
-        <v>0.36168981481481483</v>
+        <v>0.37384259259259256</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D84">
         <v>0.16</v>
@@ -4098,7 +4109,7 @@
         <v>32</v>
       </c>
       <c r="J84">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K84">
         <v>15</v>
@@ -4109,38 +4120,38 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>44848</v>
+        <v>44861</v>
       </c>
       <c r="B85" s="3">
-        <v>0.43541666666666662</v>
+        <v>0.36168981481481483</v>
       </c>
       <c r="C85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D85">
         <v>0.16</v>
       </c>
       <c r="E85">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F85">
         <f t="shared" si="4"/>
-        <v>0.25600000000000001</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G85" t="s">
         <v>7</v>
       </c>
       <c r="H85" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I85" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J85">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K85">
-        <v>16.666699999999999</v>
+        <v>15</v>
       </c>
       <c r="L85" t="s">
         <v>39</v>
@@ -4151,10 +4162,10 @@
         <v>44848</v>
       </c>
       <c r="B86" s="3">
-        <v>0.4291666666666667</v>
+        <v>0.43541666666666662</v>
       </c>
       <c r="C86" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D86">
         <v>0.16</v>
@@ -4176,7 +4187,7 @@
         <v>34</v>
       </c>
       <c r="J86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K86">
         <v>16.666699999999999</v>
@@ -4190,10 +4201,10 @@
         <v>44848</v>
       </c>
       <c r="B87" s="3">
-        <v>0.42222222222222222</v>
+        <v>0.4291666666666667</v>
       </c>
       <c r="C87" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D87">
         <v>0.16</v>
@@ -4215,7 +4226,7 @@
         <v>34</v>
       </c>
       <c r="J87">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K87">
         <v>16.666699999999999</v>
@@ -4229,10 +4240,10 @@
         <v>44848</v>
       </c>
       <c r="B88" s="3">
-        <v>0.40972222222222227</v>
+        <v>0.42222222222222222</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D88">
         <v>0.16</v>
@@ -4254,7 +4265,7 @@
         <v>34</v>
       </c>
       <c r="J88">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K88">
         <v>16.666699999999999</v>
@@ -4268,10 +4279,10 @@
         <v>44848</v>
       </c>
       <c r="B89" s="3">
-        <v>0.44236111111111115</v>
+        <v>0.40972222222222227</v>
       </c>
       <c r="C89" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D89">
         <v>0.16</v>
@@ -4293,7 +4304,7 @@
         <v>34</v>
       </c>
       <c r="J89">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K89">
         <v>16.666699999999999</v>
@@ -4307,20 +4318,20 @@
         <v>44848</v>
       </c>
       <c r="B90" s="3">
-        <v>0.38194444444444442</v>
+        <v>0.44236111111111115</v>
       </c>
       <c r="C90" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D90">
         <v>0.16</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F90">
         <f t="shared" si="4"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="G90" t="s">
         <v>7</v>
@@ -4329,10 +4340,10 @@
         <v>33</v>
       </c>
       <c r="I90" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J90">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K90">
         <v>16.666699999999999</v>
@@ -4346,10 +4357,10 @@
         <v>44848</v>
       </c>
       <c r="B91" s="3">
-        <v>0.37719907407407405</v>
+        <v>0.38194444444444442</v>
       </c>
       <c r="C91" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D91">
         <v>0.16</v>
@@ -4371,7 +4382,7 @@
         <v>32</v>
       </c>
       <c r="J91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K91">
         <v>16.666699999999999</v>
@@ -4385,10 +4396,10 @@
         <v>44848</v>
       </c>
       <c r="B92" s="3">
-        <v>0.37152777777777773</v>
+        <v>0.37719907407407405</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D92">
         <v>0.16</v>
@@ -4410,7 +4421,7 @@
         <v>32</v>
       </c>
       <c r="J92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K92">
         <v>16.666699999999999</v>
@@ -4424,10 +4435,10 @@
         <v>44848</v>
       </c>
       <c r="B93" s="3">
-        <v>0.3666666666666667</v>
+        <v>0.37152777777777773</v>
       </c>
       <c r="C93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D93">
         <v>0.16</v>
@@ -4449,13 +4460,13 @@
         <v>32</v>
       </c>
       <c r="J93">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K93">
         <v>16.666699999999999</v>
       </c>
       <c r="L93" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -4463,10 +4474,10 @@
         <v>44848</v>
       </c>
       <c r="B94" s="3">
-        <v>0.36249999999999999</v>
+        <v>0.3666666666666667</v>
       </c>
       <c r="C94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D94">
         <v>0.16</v>
@@ -4488,49 +4499,49 @@
         <v>32</v>
       </c>
       <c r="J94">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K94">
         <v>16.666699999999999</v>
       </c>
       <c r="L94" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>44845</v>
+        <v>44848</v>
       </c>
       <c r="B95" s="3">
-        <v>0.37708333333333338</v>
+        <v>0.36249999999999999</v>
       </c>
       <c r="C95" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D95">
         <v>0.16</v>
       </c>
       <c r="E95">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F95">
         <f t="shared" si="4"/>
-        <v>0.128</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G95" t="s">
         <v>7</v>
       </c>
       <c r="H95" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I95" t="s">
         <v>32</v>
       </c>
       <c r="J95">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K95">
-        <v>17.777799999999999</v>
+        <v>16.666699999999999</v>
       </c>
       <c r="L95" t="s">
         <v>39</v>
@@ -4541,10 +4552,10 @@
         <v>44845</v>
       </c>
       <c r="B96" s="3">
-        <v>0.38750000000000001</v>
+        <v>0.37708333333333338</v>
       </c>
       <c r="C96" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D96">
         <v>0.16</v>
@@ -4566,13 +4577,13 @@
         <v>32</v>
       </c>
       <c r="J96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K96">
         <v>17.777799999999999</v>
       </c>
       <c r="L96" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
@@ -4580,10 +4591,10 @@
         <v>44845</v>
       </c>
       <c r="B97" s="3">
-        <v>0.39583333333333331</v>
+        <v>0.38750000000000001</v>
       </c>
       <c r="C97" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D97">
         <v>0.16</v>
@@ -4605,13 +4616,13 @@
         <v>32</v>
       </c>
       <c r="J97">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K97">
         <v>17.777799999999999</v>
       </c>
       <c r="L97" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
@@ -4619,10 +4630,10 @@
         <v>44845</v>
       </c>
       <c r="B98" s="3">
-        <v>0.40347222222222223</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C98" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D98">
         <v>0.16</v>
@@ -4644,7 +4655,7 @@
         <v>32</v>
       </c>
       <c r="J98">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K98">
         <v>17.777799999999999</v>
@@ -4658,10 +4669,10 @@
         <v>44845</v>
       </c>
       <c r="B99" s="3">
-        <v>0.41180555555555554</v>
+        <v>0.40347222222222223</v>
       </c>
       <c r="C99" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D99">
         <v>0.16</v>
@@ -4683,52 +4694,52 @@
         <v>32</v>
       </c>
       <c r="J99">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K99">
         <v>17.777799999999999</v>
       </c>
       <c r="L99" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>44878</v>
-      </c>
-      <c r="B100" s="2">
-        <v>0.58796296296296291</v>
+        <v>44845</v>
+      </c>
+      <c r="B100" s="3">
+        <v>0.41180555555555554</v>
       </c>
       <c r="C100" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="D100">
         <v>0.16</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F100">
         <f t="shared" si="4"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.128</v>
       </c>
       <c r="G100" t="s">
         <v>7</v>
       </c>
       <c r="H100" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="I100" t="s">
         <v>32</v>
       </c>
       <c r="J100">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K100">
-        <v>11.1111</v>
+        <v>17.777799999999999</v>
       </c>
       <c r="L100" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.25">
@@ -4736,10 +4747,10 @@
         <v>44878</v>
       </c>
       <c r="B101" s="2">
-        <v>0.59398148148148155</v>
+        <v>0.58796296296296291</v>
       </c>
       <c r="C101" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D101">
         <v>0.16</v>
@@ -4761,7 +4772,7 @@
         <v>32</v>
       </c>
       <c r="J101">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K101">
         <v>11.1111</v>
@@ -4775,10 +4786,10 @@
         <v>44878</v>
       </c>
       <c r="B102" s="2">
-        <v>0.58032407407407405</v>
+        <v>0.59398148148148155</v>
       </c>
       <c r="C102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D102">
         <v>0.16</v>
@@ -4800,7 +4811,7 @@
         <v>32</v>
       </c>
       <c r="J102">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K102">
         <v>11.1111</v>
@@ -4814,10 +4825,10 @@
         <v>44878</v>
       </c>
       <c r="B103" s="2">
-        <v>0.57407407407407407</v>
+        <v>0.58032407407407405</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D103">
         <v>0.16</v>
@@ -4839,7 +4850,7 @@
         <v>32</v>
       </c>
       <c r="J103">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K103">
         <v>11.1111</v>
@@ -4853,10 +4864,10 @@
         <v>44878</v>
       </c>
       <c r="B104" s="2">
-        <v>0.56712962962962965</v>
+        <v>0.57407407407407407</v>
       </c>
       <c r="C104" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D104">
         <v>0.16</v>
@@ -4865,7 +4876,7 @@
         <v>1</v>
       </c>
       <c r="F104">
-        <f t="shared" ref="F104:F119" si="5">E104*0.064</f>
+        <f t="shared" si="4"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="G104" t="s">
@@ -4878,7 +4889,7 @@
         <v>32</v>
       </c>
       <c r="J104">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K104">
         <v>11.1111</v>
@@ -4889,38 +4900,38 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>44880</v>
+        <v>44878</v>
       </c>
       <c r="B105" s="2">
-        <v>0.4225694444444445</v>
+        <v>0.56712962962962965</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D105">
         <v>0.16</v>
       </c>
       <c r="E105">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F105">
-        <f t="shared" si="5"/>
-        <v>0.128</v>
+        <f t="shared" ref="F105:F120" si="5">E105*0.064</f>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="G105" t="s">
         <v>7</v>
       </c>
       <c r="H105" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I105" t="s">
         <v>32</v>
       </c>
       <c r="J105">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K105">
-        <v>6.6666699999999999</v>
+        <v>11.1111</v>
       </c>
       <c r="L105" t="s">
         <v>39</v>
@@ -4931,10 +4942,10 @@
         <v>44880</v>
       </c>
       <c r="B106" s="2">
-        <v>0.42777777777777781</v>
+        <v>0.4225694444444445</v>
       </c>
       <c r="C106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D106">
         <v>0.16</v>
@@ -4956,7 +4967,7 @@
         <v>32</v>
       </c>
       <c r="J106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K106">
         <v>6.6666699999999999</v>
@@ -4970,10 +4981,10 @@
         <v>44880</v>
       </c>
       <c r="B107" s="2">
-        <v>0.43402777777777773</v>
+        <v>0.42777777777777781</v>
       </c>
       <c r="C107" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D107">
         <v>0.16</v>
@@ -4995,7 +5006,7 @@
         <v>32</v>
       </c>
       <c r="J107">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K107">
         <v>6.6666699999999999</v>
@@ -5009,10 +5020,10 @@
         <v>44880</v>
       </c>
       <c r="B108" s="2">
-        <v>0.4513888888888889</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="C108" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D108">
         <v>0.16</v>
@@ -5034,13 +5045,13 @@
         <v>32</v>
       </c>
       <c r="J108">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K108">
         <v>6.6666699999999999</v>
       </c>
       <c r="L108" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -5048,10 +5059,10 @@
         <v>44880</v>
       </c>
       <c r="B109" s="2">
-        <v>0.45763888888888887</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D109">
         <v>0.16</v>
@@ -5073,49 +5084,49 @@
         <v>32</v>
       </c>
       <c r="J109">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K109">
         <v>6.6666699999999999</v>
       </c>
       <c r="L109" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>44882</v>
+        <v>44880</v>
       </c>
       <c r="B110" s="2">
-        <v>0.52638888888888891</v>
+        <v>0.45763888888888887</v>
       </c>
       <c r="C110" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D110">
         <v>0.16</v>
       </c>
       <c r="E110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F110">
         <f t="shared" si="5"/>
-        <v>0.192</v>
+        <v>0.128</v>
       </c>
       <c r="G110" t="s">
         <v>7</v>
       </c>
       <c r="H110" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I110" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J110">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K110">
-        <v>8.88889</v>
+        <v>6.6666699999999999</v>
       </c>
       <c r="L110" t="s">
         <v>39</v>
@@ -5126,20 +5137,20 @@
         <v>44882</v>
       </c>
       <c r="B111" s="2">
-        <v>0.53680555555555554</v>
+        <v>0.52638888888888891</v>
       </c>
       <c r="C111" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D111">
         <v>0.16</v>
       </c>
       <c r="E111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F111">
         <f t="shared" si="5"/>
-        <v>0.25600000000000001</v>
+        <v>0.192</v>
       </c>
       <c r="G111" t="s">
         <v>7</v>
@@ -5151,7 +5162,7 @@
         <v>34</v>
       </c>
       <c r="J111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K111">
         <v>8.88889</v>
@@ -5165,20 +5176,20 @@
         <v>44882</v>
       </c>
       <c r="B112" s="2">
-        <v>0.5444444444444444</v>
+        <v>0.53680555555555554</v>
       </c>
       <c r="C112" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D112">
         <v>0.16</v>
       </c>
       <c r="E112">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F112">
         <f t="shared" si="5"/>
-        <v>0.192</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="G112" t="s">
         <v>7</v>
@@ -5190,7 +5201,7 @@
         <v>34</v>
       </c>
       <c r="J112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K112">
         <v>8.88889</v>
@@ -5204,10 +5215,10 @@
         <v>44882</v>
       </c>
       <c r="B113" s="2">
-        <v>0.55277777777777781</v>
+        <v>0.5444444444444444</v>
       </c>
       <c r="C113" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D113">
         <v>0.16</v>
@@ -5229,7 +5240,7 @@
         <v>34</v>
       </c>
       <c r="J113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K113">
         <v>8.88889</v>
@@ -5243,10 +5254,10 @@
         <v>44882</v>
       </c>
       <c r="B114" s="2">
-        <v>0.56666666666666665</v>
+        <v>0.55277777777777781</v>
       </c>
       <c r="C114" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D114">
         <v>0.16</v>
@@ -5268,13 +5279,13 @@
         <v>34</v>
       </c>
       <c r="J114">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K114">
         <v>8.88889</v>
       </c>
       <c r="L114" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
@@ -5282,20 +5293,20 @@
         <v>44882</v>
       </c>
       <c r="B115" s="2">
-        <v>0.48749999999999999</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="C115" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D115">
         <v>0.16</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F115">
         <f t="shared" si="5"/>
-        <v>6.4000000000000001E-2</v>
+        <v>0.192</v>
       </c>
       <c r="G115" t="s">
         <v>7</v>
@@ -5304,16 +5315,16 @@
         <v>33</v>
       </c>
       <c r="I115" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J115">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K115">
-        <v>7.7777799999999999</v>
+        <v>8.88889</v>
       </c>
       <c r="L115" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
@@ -5321,10 +5332,10 @@
         <v>44882</v>
       </c>
       <c r="B116" s="2">
-        <v>0.4513888888888889</v>
+        <v>0.48749999999999999</v>
       </c>
       <c r="C116" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D116">
         <v>0.16</v>
@@ -5346,13 +5357,13 @@
         <v>32</v>
       </c>
       <c r="J116">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K116">
         <v>7.7777799999999999</v>
       </c>
       <c r="L116" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
@@ -5360,10 +5371,10 @@
         <v>44882</v>
       </c>
       <c r="B117" s="2">
-        <v>0.4597222222222222</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="C117" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D117">
         <v>0.16</v>
@@ -5385,7 +5396,7 @@
         <v>32</v>
       </c>
       <c r="J117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K117">
         <v>7.7777799999999999</v>
@@ -5399,10 +5410,10 @@
         <v>44882</v>
       </c>
       <c r="B118" s="2">
-        <v>0.47569444444444442</v>
+        <v>0.4597222222222222</v>
       </c>
       <c r="C118" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D118">
         <v>0.16</v>
@@ -5424,7 +5435,7 @@
         <v>32</v>
       </c>
       <c r="J118">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K118">
         <v>7.7777799999999999</v>
@@ -5438,10 +5449,10 @@
         <v>44882</v>
       </c>
       <c r="B119" s="2">
-        <v>0.46736111111111112</v>
+        <v>0.47569444444444442</v>
       </c>
       <c r="C119" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D119">
         <v>0.16</v>
@@ -5463,12 +5474,51 @@
         <v>32</v>
       </c>
       <c r="J119">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K119">
         <v>7.7777799999999999</v>
       </c>
       <c r="L119" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44882</v>
+      </c>
+      <c r="B120" s="2">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="C120" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120">
+        <v>0.16</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="5"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G120" t="s">
+        <v>7</v>
+      </c>
+      <c r="H120" t="s">
+        <v>33</v>
+      </c>
+      <c r="I120" t="s">
+        <v>32</v>
+      </c>
+      <c r="J120">
+        <v>5</v>
+      </c>
+      <c r="K120">
+        <v>7.7777799999999999</v>
+      </c>
+      <c r="L120" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add default (in Quarto params) and custom (in metadata) dead bands
See #6
</commit_message>
<xml_diff>
--- a/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
+++ b/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Biogeochemistry\People\Wilson (Steph)\Data\Fluxes\Chamber Fluxes\Data for Ben\All_2022_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpbond/Dropbox/Mac/Documents/Code/sw/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9775C0C-90B4-4380-95E2-878CFBABCDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7693A1-932F-B042-B026-AE00C33E4DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="45" windowWidth="16155" windowHeight="11340" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="16160" windowHeight="11340" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPASS_ChamberFlux_Metadata_20" sheetId="1" r:id="rId1"/>
@@ -37,6 +37,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>User</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{13733613-97D8-F84A-9018-6142D67C8148}">
@@ -102,7 +103,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -111,12 +112,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Plot ID</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Plot ID</t>
         </r>
       </text>
     </comment>
@@ -193,7 +203,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -202,12 +212,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Total volume of chambers, in m2</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Total volume of chambers, in m2</t>
         </r>
       </text>
     </comment>
@@ -217,7 +236,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -226,12 +245,54 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Light level of flux: Dark, Full, Half, or Quarter</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Light level of flux: Dark, Full, Half, or Quarter</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="1" shapeId="0" xr:uid="{681BEF99-CFE0-EA4D-B797-603D99F71A0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Custom dead band time, seconds</t>
         </r>
       </text>
     </comment>
@@ -240,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="66">
   <si>
     <t>Date</t>
   </si>
@@ -432,6 +493,12 @@
   </si>
   <si>
     <t xml:space="preserve">different grass spp than other 4 </t>
+  </si>
+  <si>
+    <t>Dead_band</t>
+  </si>
+  <si>
+    <t>CO2 and CH4 have big discontinuity (drop) at ~50 seconds</t>
   </si>
 </sst>
 </file>
@@ -441,7 +508,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -488,6 +555,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -509,15 +589,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -832,19 +910,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5B7D07-181D-BE46-BEC5-DBDE824ED711}">
-  <dimension ref="A1:L120"/>
+  <dimension ref="A1:M120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
-    <col min="3" max="3" width="14.625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -878,11 +957,14 @@
       <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44718</v>
       </c>
@@ -917,11 +999,11 @@
       <c r="K2">
         <v>21.666699999999999</v>
       </c>
-      <c r="L2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44718</v>
       </c>
@@ -956,11 +1038,11 @@
       <c r="K3">
         <v>21.666699999999999</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44718</v>
       </c>
@@ -995,11 +1077,11 @@
       <c r="K4">
         <v>21.666699999999999</v>
       </c>
-      <c r="L4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44718</v>
       </c>
@@ -1034,11 +1116,11 @@
       <c r="K5">
         <v>21.666699999999999</v>
       </c>
-      <c r="L5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44721</v>
       </c>
@@ -1073,11 +1155,11 @@
       <c r="K6">
         <v>25.555599999999998</v>
       </c>
-      <c r="L6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44721</v>
       </c>
@@ -1112,11 +1194,11 @@
       <c r="K7">
         <v>25.555599999999998</v>
       </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44721</v>
       </c>
@@ -1151,11 +1233,11 @@
       <c r="K8">
         <v>25.555599999999998</v>
       </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44721</v>
       </c>
@@ -1190,11 +1272,11 @@
       <c r="K9">
         <v>25.555599999999998</v>
       </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44721</v>
       </c>
@@ -1229,11 +1311,11 @@
       <c r="K10">
         <v>25.555599999999998</v>
       </c>
-      <c r="L10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44721</v>
       </c>
@@ -1268,11 +1350,14 @@
       <c r="K11">
         <v>25.555599999999998</v>
       </c>
-      <c r="L11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="5">
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44721</v>
       </c>
@@ -1307,11 +1392,11 @@
       <c r="K12">
         <v>25.555599999999998</v>
       </c>
-      <c r="L12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44721</v>
       </c>
@@ -1346,11 +1431,11 @@
       <c r="K13">
         <v>25.555599999999998</v>
       </c>
-      <c r="L13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44721</v>
       </c>
@@ -1385,11 +1470,11 @@
       <c r="K14">
         <v>25.555599999999998</v>
       </c>
-      <c r="L14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44721</v>
       </c>
@@ -1424,11 +1509,11 @@
       <c r="K15">
         <v>25.555599999999998</v>
       </c>
-      <c r="L15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44722</v>
       </c>
@@ -1463,11 +1548,11 @@
       <c r="K16">
         <v>24.444400000000002</v>
       </c>
-      <c r="L16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44722</v>
       </c>
@@ -1502,11 +1587,11 @@
       <c r="K17">
         <v>24.444400000000002</v>
       </c>
-      <c r="L17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44722</v>
       </c>
@@ -1541,11 +1626,11 @@
       <c r="K18">
         <v>24.444400000000002</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44722</v>
       </c>
@@ -1580,11 +1665,11 @@
       <c r="K19">
         <v>24.444400000000002</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44722</v>
       </c>
@@ -1619,11 +1704,11 @@
       <c r="K20">
         <v>24.444400000000002</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44756</v>
       </c>
@@ -1657,11 +1742,11 @@
       <c r="K21">
         <v>30</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44756</v>
       </c>
@@ -1696,11 +1781,11 @@
       <c r="K22">
         <v>30</v>
       </c>
-      <c r="L22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44756</v>
       </c>
@@ -1735,11 +1820,11 @@
       <c r="K23">
         <v>30</v>
       </c>
-      <c r="L23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44756</v>
       </c>
@@ -1774,11 +1859,11 @@
       <c r="K24">
         <v>30</v>
       </c>
-      <c r="L24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44756</v>
       </c>
@@ -1813,11 +1898,11 @@
       <c r="K25">
         <v>30</v>
       </c>
-      <c r="L25" t="s">
+      <c r="M25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44754</v>
       </c>
@@ -1852,11 +1937,11 @@
       <c r="K26">
         <v>29.444400000000002</v>
       </c>
-      <c r="L26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44754</v>
       </c>
@@ -1891,11 +1976,11 @@
       <c r="K27">
         <v>29.444400000000002</v>
       </c>
-      <c r="L27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44754</v>
       </c>
@@ -1930,11 +2015,11 @@
       <c r="K28">
         <v>29.444400000000002</v>
       </c>
-      <c r="L28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44754</v>
       </c>
@@ -1969,11 +2054,11 @@
       <c r="K29">
         <v>29.444400000000002</v>
       </c>
-      <c r="L29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44754</v>
       </c>
@@ -2008,11 +2093,11 @@
       <c r="K30">
         <v>29.444400000000002</v>
       </c>
-      <c r="L30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44754</v>
       </c>
@@ -2047,11 +2132,11 @@
       <c r="K31">
         <v>29.444400000000002</v>
       </c>
-      <c r="L31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44754</v>
       </c>
@@ -2086,11 +2171,11 @@
       <c r="K32">
         <v>29.444400000000002</v>
       </c>
-      <c r="L32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44754</v>
       </c>
@@ -2125,11 +2210,11 @@
       <c r="K33">
         <v>29.444400000000002</v>
       </c>
-      <c r="L33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44754</v>
       </c>
@@ -2164,11 +2249,11 @@
       <c r="K34">
         <v>29.444400000000002</v>
       </c>
-      <c r="L34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44754</v>
       </c>
@@ -2203,206 +2288,206 @@
       <c r="K35">
         <v>29.444400000000002</v>
       </c>
-      <c r="L35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+      <c r="M35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
         <v>44753</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="3">
         <v>0.3840277777777778</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E36" s="7">
-        <v>2</v>
-      </c>
-      <c r="F36" s="7">
+      <c r="D36">
+        <v>0.16</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="7" t="s">
+      <c r="G36" t="s">
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J36" s="7">
-        <v>1</v>
-      </c>
-      <c r="K36" s="7">
+      <c r="I36" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+      <c r="K36">
         <v>30</v>
       </c>
-      <c r="L36" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="M36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
         <v>44753</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="3">
         <v>0.39444444444444443</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E37" s="7">
-        <v>2</v>
-      </c>
-      <c r="F37" s="7">
+      <c r="D37">
+        <v>0.16</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H37" s="7" t="s">
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" t="s">
         <v>35</v>
       </c>
-      <c r="I37" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J37" s="7">
-        <v>2</v>
-      </c>
-      <c r="K37" s="7">
+      <c r="I37" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37">
+        <v>2</v>
+      </c>
+      <c r="K37">
         <v>30</v>
       </c>
-      <c r="L37" s="7" t="s">
+      <c r="M37" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
         <v>44753</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="3">
         <v>0.40277777777777773</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E38" s="7">
-        <v>2</v>
-      </c>
-      <c r="F38" s="7">
+      <c r="D38">
+        <v>0.16</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="7" t="s">
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" t="s">
         <v>35</v>
       </c>
-      <c r="I38" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J38" s="7">
+      <c r="I38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38">
         <v>3</v>
       </c>
-      <c r="K38" s="7">
+      <c r="K38">
         <v>30</v>
       </c>
-      <c r="L38" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="M38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
         <v>44753</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="3">
         <v>0.40972222222222227</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E39" s="7">
-        <v>2</v>
-      </c>
-      <c r="F39" s="7">
+      <c r="D39">
+        <v>0.16</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H39" s="7" t="s">
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" t="s">
         <v>35</v>
       </c>
-      <c r="I39" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J39" s="7">
+      <c r="I39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39">
         <v>4</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39">
         <v>30</v>
       </c>
-      <c r="L39" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="M39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
         <v>44753</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="3">
         <v>0.41666666666666669</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="7">
-        <v>0.16</v>
-      </c>
-      <c r="E40" s="7">
-        <v>2</v>
-      </c>
-      <c r="F40" s="7">
+      <c r="D40">
+        <v>0.16</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="1"/>
         <v>0.128</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="7" t="s">
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" t="s">
         <v>35</v>
       </c>
-      <c r="I40" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J40" s="7">
+      <c r="I40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40">
         <v>5</v>
       </c>
-      <c r="K40" s="7">
+      <c r="K40">
         <v>30</v>
       </c>
-      <c r="L40" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44804</v>
       </c>
@@ -2437,11 +2522,11 @@
       <c r="K41">
         <v>27.2</v>
       </c>
-      <c r="L41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44804</v>
       </c>
@@ -2476,11 +2561,11 @@
       <c r="K42">
         <v>27.2</v>
       </c>
-      <c r="L42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44804</v>
       </c>
@@ -2515,11 +2600,11 @@
       <c r="K43">
         <v>27.2</v>
       </c>
-      <c r="L43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44804</v>
       </c>
@@ -2554,11 +2639,11 @@
       <c r="K44">
         <v>27.2</v>
       </c>
-      <c r="L44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44804</v>
       </c>
@@ -2593,11 +2678,11 @@
       <c r="K45">
         <v>27.2</v>
       </c>
-      <c r="L45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44791</v>
       </c>
@@ -2632,11 +2717,11 @@
       <c r="K46">
         <v>29.5</v>
       </c>
-      <c r="L46" t="s">
+      <c r="M46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44791</v>
       </c>
@@ -2671,11 +2756,11 @@
       <c r="K47">
         <v>29.5</v>
       </c>
-      <c r="L47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44791</v>
       </c>
@@ -2710,11 +2795,11 @@
       <c r="K48">
         <v>29.5</v>
       </c>
-      <c r="L48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44791</v>
       </c>
@@ -2749,11 +2834,11 @@
       <c r="K49">
         <v>29.5</v>
       </c>
-      <c r="L49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>44791</v>
       </c>
@@ -2788,11 +2873,11 @@
       <c r="K50">
         <v>29.5</v>
       </c>
-      <c r="L50" t="s">
+      <c r="M50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44791</v>
       </c>
@@ -2827,11 +2912,11 @@
       <c r="K51">
         <v>29.5</v>
       </c>
-      <c r="L51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>44791</v>
       </c>
@@ -2866,11 +2951,11 @@
       <c r="K52">
         <v>29.5</v>
       </c>
-      <c r="L52" t="s">
+      <c r="M52" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44791</v>
       </c>
@@ -2905,11 +2990,11 @@
       <c r="K53">
         <v>29.5</v>
       </c>
-      <c r="L53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>44791</v>
       </c>
@@ -2944,11 +3029,11 @@
       <c r="K54">
         <v>29.5</v>
       </c>
-      <c r="L54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>44791</v>
       </c>
@@ -2983,11 +3068,11 @@
       <c r="K55">
         <v>29.5</v>
       </c>
-      <c r="L55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>44788</v>
       </c>
@@ -3022,11 +3107,11 @@
       <c r="K56">
         <v>28.8</v>
       </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>44788</v>
       </c>
@@ -3061,11 +3146,11 @@
       <c r="K57">
         <v>28.8</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>44788</v>
       </c>
@@ -3100,11 +3185,11 @@
       <c r="K58">
         <v>28.8</v>
       </c>
-      <c r="L58" t="s">
+      <c r="M58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>44788</v>
       </c>
@@ -3139,11 +3224,11 @@
       <c r="K59">
         <v>28.8</v>
       </c>
-      <c r="L59" t="s">
+      <c r="M59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>44788</v>
       </c>
@@ -3178,11 +3263,11 @@
       <c r="K60">
         <v>28.8</v>
       </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>44822</v>
       </c>
@@ -3217,11 +3302,11 @@
       <c r="K61">
         <v>20.100000000000001</v>
       </c>
-      <c r="L61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>44822</v>
       </c>
@@ -3256,11 +3341,11 @@
       <c r="K62">
         <v>20.100000000000001</v>
       </c>
-      <c r="L62" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44822</v>
       </c>
@@ -3295,11 +3380,11 @@
       <c r="K63">
         <v>20.100000000000001</v>
       </c>
-      <c r="L63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>44822</v>
       </c>
@@ -3334,11 +3419,11 @@
       <c r="K64">
         <v>20.100000000000001</v>
       </c>
-      <c r="L64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44822</v>
       </c>
@@ -3373,11 +3458,11 @@
       <c r="K65">
         <v>20.100000000000001</v>
       </c>
-      <c r="L65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>44826</v>
       </c>
@@ -3412,11 +3497,11 @@
       <c r="K66">
         <v>28.332999999999998</v>
       </c>
-      <c r="L66" t="s">
+      <c r="M66" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>44826</v>
       </c>
@@ -3451,11 +3536,11 @@
       <c r="K67">
         <v>28.332999999999998</v>
       </c>
-      <c r="L67" t="s">
+      <c r="M67" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>44826</v>
       </c>
@@ -3490,11 +3575,11 @@
       <c r="K68">
         <v>28.332999999999998</v>
       </c>
-      <c r="L68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>44826</v>
       </c>
@@ -3529,11 +3614,11 @@
       <c r="K69">
         <v>28.332999999999998</v>
       </c>
-      <c r="L69" t="s">
+      <c r="M69" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>44826</v>
       </c>
@@ -3568,11 +3653,11 @@
       <c r="K70">
         <v>28.332999999999998</v>
       </c>
-      <c r="L70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>44826</v>
       </c>
@@ -3607,11 +3692,11 @@
       <c r="K71">
         <v>26.111000000000001</v>
       </c>
-      <c r="L71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>44826</v>
       </c>
@@ -3646,11 +3731,11 @@
       <c r="K72">
         <v>26.111000000000001</v>
       </c>
-      <c r="L72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44826</v>
       </c>
@@ -3685,11 +3770,11 @@
       <c r="K73">
         <v>26.111000000000001</v>
       </c>
-      <c r="L73" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44826</v>
       </c>
@@ -3724,11 +3809,11 @@
       <c r="K74">
         <v>26.111000000000001</v>
       </c>
-      <c r="L74" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44826</v>
       </c>
@@ -3763,11 +3848,11 @@
       <c r="K75">
         <v>26.111000000000001</v>
       </c>
-      <c r="L75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44823</v>
       </c>
@@ -3802,11 +3887,11 @@
       <c r="K76">
         <v>28.332999999999998</v>
       </c>
-      <c r="L76" t="s">
+      <c r="M76" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44823</v>
       </c>
@@ -3841,11 +3926,11 @@
       <c r="K77">
         <v>28.332999999999998</v>
       </c>
-      <c r="L77" t="s">
+      <c r="M77" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44823</v>
       </c>
@@ -3880,11 +3965,11 @@
       <c r="K78">
         <v>28.332999999999998</v>
       </c>
-      <c r="L78" t="s">
+      <c r="M78" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44823</v>
       </c>
@@ -3919,11 +4004,11 @@
       <c r="K79">
         <v>28.332999999999998</v>
       </c>
-      <c r="L79" t="s">
+      <c r="M79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44823</v>
       </c>
@@ -3958,11 +4043,11 @@
       <c r="K80">
         <v>28.332999999999998</v>
       </c>
-      <c r="L80" t="s">
+      <c r="M80" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44861</v>
       </c>
@@ -3997,11 +4082,11 @@
       <c r="K81">
         <v>15</v>
       </c>
-      <c r="L81" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44861</v>
       </c>
@@ -4036,11 +4121,11 @@
       <c r="K82">
         <v>15</v>
       </c>
-      <c r="L82" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44861</v>
       </c>
@@ -4075,11 +4160,11 @@
       <c r="K83">
         <v>15</v>
       </c>
-      <c r="L83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44861</v>
       </c>
@@ -4114,11 +4199,11 @@
       <c r="K84">
         <v>15</v>
       </c>
-      <c r="L84" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44861</v>
       </c>
@@ -4153,11 +4238,11 @@
       <c r="K85">
         <v>15</v>
       </c>
-      <c r="L85" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44848</v>
       </c>
@@ -4192,11 +4277,11 @@
       <c r="K86">
         <v>16.666699999999999</v>
       </c>
-      <c r="L86" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44848</v>
       </c>
@@ -4231,11 +4316,11 @@
       <c r="K87">
         <v>16.666699999999999</v>
       </c>
-      <c r="L87" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44848</v>
       </c>
@@ -4270,11 +4355,11 @@
       <c r="K88">
         <v>16.666699999999999</v>
       </c>
-      <c r="L88" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44848</v>
       </c>
@@ -4309,11 +4394,11 @@
       <c r="K89">
         <v>16.666699999999999</v>
       </c>
-      <c r="L89" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44848</v>
       </c>
@@ -4348,11 +4433,11 @@
       <c r="K90">
         <v>16.666699999999999</v>
       </c>
-      <c r="L90" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44848</v>
       </c>
@@ -4387,11 +4472,11 @@
       <c r="K91">
         <v>16.666699999999999</v>
       </c>
-      <c r="L91" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44848</v>
       </c>
@@ -4426,11 +4511,11 @@
       <c r="K92">
         <v>16.666699999999999</v>
       </c>
-      <c r="L92" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44848</v>
       </c>
@@ -4465,11 +4550,11 @@
       <c r="K93">
         <v>16.666699999999999</v>
       </c>
-      <c r="L93" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44848</v>
       </c>
@@ -4504,11 +4589,11 @@
       <c r="K94">
         <v>16.666699999999999</v>
       </c>
-      <c r="L94" t="s">
+      <c r="M94" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44848</v>
       </c>
@@ -4543,11 +4628,11 @@
       <c r="K95">
         <v>16.666699999999999</v>
       </c>
-      <c r="L95" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44845</v>
       </c>
@@ -4582,11 +4667,11 @@
       <c r="K96">
         <v>17.777799999999999</v>
       </c>
-      <c r="L96" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44845</v>
       </c>
@@ -4621,11 +4706,11 @@
       <c r="K97">
         <v>17.777799999999999</v>
       </c>
-      <c r="L97" t="s">
+      <c r="M97" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44845</v>
       </c>
@@ -4660,11 +4745,11 @@
       <c r="K98">
         <v>17.777799999999999</v>
       </c>
-      <c r="L98" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44845</v>
       </c>
@@ -4699,11 +4784,11 @@
       <c r="K99">
         <v>17.777799999999999</v>
       </c>
-      <c r="L99" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>44845</v>
       </c>
@@ -4738,11 +4823,11 @@
       <c r="K100">
         <v>17.777799999999999</v>
       </c>
-      <c r="L100" t="s">
+      <c r="M100" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44878</v>
       </c>
@@ -4777,11 +4862,11 @@
       <c r="K101">
         <v>11.1111</v>
       </c>
-      <c r="L101" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>44878</v>
       </c>
@@ -4816,11 +4901,11 @@
       <c r="K102">
         <v>11.1111</v>
       </c>
-      <c r="L102" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>44878</v>
       </c>
@@ -4855,11 +4940,11 @@
       <c r="K103">
         <v>11.1111</v>
       </c>
-      <c r="L103" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M103" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>44878</v>
       </c>
@@ -4894,11 +4979,11 @@
       <c r="K104">
         <v>11.1111</v>
       </c>
-      <c r="L104" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M104" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>44878</v>
       </c>
@@ -4933,11 +5018,11 @@
       <c r="K105">
         <v>11.1111</v>
       </c>
-      <c r="L105" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M105" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>44880</v>
       </c>
@@ -4972,11 +5057,11 @@
       <c r="K106">
         <v>6.6666699999999999</v>
       </c>
-      <c r="L106" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>44880</v>
       </c>
@@ -5011,11 +5096,11 @@
       <c r="K107">
         <v>6.6666699999999999</v>
       </c>
-      <c r="L107" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M107" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>44880</v>
       </c>
@@ -5050,11 +5135,11 @@
       <c r="K108">
         <v>6.6666699999999999</v>
       </c>
-      <c r="L108" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M108" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>44880</v>
       </c>
@@ -5089,11 +5174,11 @@
       <c r="K109">
         <v>6.6666699999999999</v>
       </c>
-      <c r="L109" t="s">
+      <c r="M109" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>44880</v>
       </c>
@@ -5128,11 +5213,11 @@
       <c r="K110">
         <v>6.6666699999999999</v>
       </c>
-      <c r="L110" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M110" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>44882</v>
       </c>
@@ -5167,11 +5252,11 @@
       <c r="K111">
         <v>8.88889</v>
       </c>
-      <c r="L111" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M111" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>44882</v>
       </c>
@@ -5206,11 +5291,11 @@
       <c r="K112">
         <v>8.88889</v>
       </c>
-      <c r="L112" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M112" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>44882</v>
       </c>
@@ -5245,11 +5330,11 @@
       <c r="K113">
         <v>8.88889</v>
       </c>
-      <c r="L113" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M113" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>44882</v>
       </c>
@@ -5284,11 +5369,11 @@
       <c r="K114">
         <v>8.88889</v>
       </c>
-      <c r="L114" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M114" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>44882</v>
       </c>
@@ -5323,11 +5408,11 @@
       <c r="K115">
         <v>8.88889</v>
       </c>
-      <c r="L115" t="s">
+      <c r="M115" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>44882</v>
       </c>
@@ -5362,11 +5447,11 @@
       <c r="K116">
         <v>7.7777799999999999</v>
       </c>
-      <c r="L116" t="s">
+      <c r="M116" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>44882</v>
       </c>
@@ -5401,11 +5486,11 @@
       <c r="K117">
         <v>7.7777799999999999</v>
       </c>
-      <c r="L117" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>44882</v>
       </c>
@@ -5440,11 +5525,11 @@
       <c r="K118">
         <v>7.7777799999999999</v>
       </c>
-      <c r="L118" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M118" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>44882</v>
       </c>
@@ -5479,11 +5564,11 @@
       <c r="K119">
         <v>7.7777799999999999</v>
       </c>
-      <c r="L119" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M119" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>44882</v>
       </c>
@@ -5518,7 +5603,7 @@
       <c r="K120">
         <v>7.7777799999999999</v>
       </c>
-      <c r="L120" t="s">
+      <c r="M120" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add "Msmt_stop" column to metadata & code to handle
</commit_message>
<xml_diff>
--- a/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
+++ b/data/COMPASS_ChamberFlux_Metadata_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bpbond/Dropbox/Mac/Documents/Code/sw/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7693A1-932F-B042-B026-AE00C33E4DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFB43EF-87B7-1B46-A97F-9CF877FE6EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="500" windowWidth="16160" windowHeight="11340" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
+    <workbookView xWindow="1080" yWindow="500" windowWidth="24000" windowHeight="16340" xr2:uid="{43107FA4-7C6A-8A41-9858-E4BE7819DE13}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPASS_ChamberFlux_Metadata_20" sheetId="1" r:id="rId1"/>
@@ -179,7 +179,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -188,12 +188,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Number of chambers stacked during flux measurement</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of chambers stacked during flux measurement</t>
         </r>
       </text>
     </comment>
@@ -292,7 +301,41 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Custom dead band time, seconds</t>
+          <t>Custom dead band time, seconds. This column is optional.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="1" shapeId="0" xr:uid="{F4C08C31-B896-7A4D-9304-28BD7185CD19}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Custom measurement stop point, seconds since start (not including dead band). Optional.
+</t>
         </r>
       </text>
     </comment>
@@ -301,7 +344,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -499,6 +542,9 @@
   </si>
   <si>
     <t>CO2 and CH4 have big discontinuity (drop) at ~50 seconds</t>
+  </si>
+  <si>
+    <t>Msmt_stop</t>
   </si>
 </sst>
 </file>
@@ -589,13 +635,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,20 +955,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5B7D07-181D-BE46-BEC5-DBDE824ED711}">
-  <dimension ref="A1:M120"/>
+  <dimension ref="A1:N120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11" style="2"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -957,14 +1003,17 @@
       <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" t="s">
         <v>64</v>
       </c>
       <c r="M1" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44718</v>
       </c>
@@ -999,11 +1048,11 @@
       <c r="K2">
         <v>21.666699999999999</v>
       </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44718</v>
       </c>
@@ -1038,11 +1087,11 @@
       <c r="K3">
         <v>21.666699999999999</v>
       </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44718</v>
       </c>
@@ -1077,11 +1126,11 @@
       <c r="K4">
         <v>21.666699999999999</v>
       </c>
-      <c r="M4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44718</v>
       </c>
@@ -1116,11 +1165,11 @@
       <c r="K5">
         <v>21.666699999999999</v>
       </c>
-      <c r="M5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44721</v>
       </c>
@@ -1155,11 +1204,11 @@
       <c r="K6">
         <v>25.555599999999998</v>
       </c>
-      <c r="M6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44721</v>
       </c>
@@ -1194,11 +1243,11 @@
       <c r="K7">
         <v>25.555599999999998</v>
       </c>
-      <c r="M7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44721</v>
       </c>
@@ -1233,11 +1282,11 @@
       <c r="K8">
         <v>25.555599999999998</v>
       </c>
-      <c r="M8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44721</v>
       </c>
@@ -1272,11 +1321,11 @@
       <c r="K9">
         <v>25.555599999999998</v>
       </c>
-      <c r="M9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44721</v>
       </c>
@@ -1311,11 +1360,11 @@
       <c r="K10">
         <v>25.555599999999998</v>
       </c>
-      <c r="M10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44721</v>
       </c>
@@ -1350,14 +1399,17 @@
       <c r="K11">
         <v>25.555599999999998</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11">
         <v>60</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11">
+        <v>200</v>
+      </c>
+      <c r="N11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44721</v>
       </c>
@@ -1392,11 +1444,11 @@
       <c r="K12">
         <v>25.555599999999998</v>
       </c>
-      <c r="M12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44721</v>
       </c>
@@ -1431,11 +1483,11 @@
       <c r="K13">
         <v>25.555599999999998</v>
       </c>
-      <c r="M13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44721</v>
       </c>
@@ -1470,11 +1522,11 @@
       <c r="K14">
         <v>25.555599999999998</v>
       </c>
-      <c r="M14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44721</v>
       </c>
@@ -1509,11 +1561,11 @@
       <c r="K15">
         <v>25.555599999999998</v>
       </c>
-      <c r="M15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44722</v>
       </c>
@@ -1548,11 +1600,11 @@
       <c r="K16">
         <v>24.444400000000002</v>
       </c>
-      <c r="M16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44722</v>
       </c>
@@ -1587,11 +1639,11 @@
       <c r="K17">
         <v>24.444400000000002</v>
       </c>
-      <c r="M17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44722</v>
       </c>
@@ -1626,11 +1678,11 @@
       <c r="K18">
         <v>24.444400000000002</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44722</v>
       </c>
@@ -1665,11 +1717,11 @@
       <c r="K19">
         <v>24.444400000000002</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>44722</v>
       </c>
@@ -1704,11 +1756,11 @@
       <c r="K20">
         <v>24.444400000000002</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>44756</v>
       </c>
@@ -1742,11 +1794,11 @@
       <c r="K21">
         <v>30</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>44756</v>
       </c>
@@ -1781,11 +1833,11 @@
       <c r="K22">
         <v>30</v>
       </c>
-      <c r="M22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>44756</v>
       </c>
@@ -1820,11 +1872,11 @@
       <c r="K23">
         <v>30</v>
       </c>
-      <c r="M23" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>44756</v>
       </c>
@@ -1859,11 +1911,11 @@
       <c r="K24">
         <v>30</v>
       </c>
-      <c r="M24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>44756</v>
       </c>
@@ -1898,11 +1950,11 @@
       <c r="K25">
         <v>30</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>44754</v>
       </c>
@@ -1937,11 +1989,11 @@
       <c r="K26">
         <v>29.444400000000002</v>
       </c>
-      <c r="M26" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>44754</v>
       </c>
@@ -1976,11 +2028,11 @@
       <c r="K27">
         <v>29.444400000000002</v>
       </c>
-      <c r="M27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>44754</v>
       </c>
@@ -2015,11 +2067,11 @@
       <c r="K28">
         <v>29.444400000000002</v>
       </c>
-      <c r="M28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>44754</v>
       </c>
@@ -2054,11 +2106,11 @@
       <c r="K29">
         <v>29.444400000000002</v>
       </c>
-      <c r="M29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>44754</v>
       </c>
@@ -2093,11 +2145,11 @@
       <c r="K30">
         <v>29.444400000000002</v>
       </c>
-      <c r="M30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>44754</v>
       </c>
@@ -2132,11 +2184,11 @@
       <c r="K31">
         <v>29.444400000000002</v>
       </c>
-      <c r="M31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>44754</v>
       </c>
@@ -2171,11 +2223,11 @@
       <c r="K32">
         <v>29.444400000000002</v>
       </c>
-      <c r="M32" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>44754</v>
       </c>
@@ -2210,11 +2262,11 @@
       <c r="K33">
         <v>29.444400000000002</v>
       </c>
-      <c r="M33" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>44754</v>
       </c>
@@ -2249,11 +2301,11 @@
       <c r="K34">
         <v>29.444400000000002</v>
       </c>
-      <c r="M34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>44754</v>
       </c>
@@ -2288,11 +2340,11 @@
       <c r="K35">
         <v>29.444400000000002</v>
       </c>
-      <c r="M35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>44753</v>
       </c>
@@ -2327,11 +2379,11 @@
       <c r="K36">
         <v>30</v>
       </c>
-      <c r="M36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>44753</v>
       </c>
@@ -2366,11 +2418,11 @@
       <c r="K37">
         <v>30</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>44753</v>
       </c>
@@ -2405,11 +2457,11 @@
       <c r="K38">
         <v>30</v>
       </c>
-      <c r="M38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>44753</v>
       </c>
@@ -2444,11 +2496,11 @@
       <c r="K39">
         <v>30</v>
       </c>
-      <c r="M39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>44753</v>
       </c>
@@ -2483,11 +2535,11 @@
       <c r="K40">
         <v>30</v>
       </c>
-      <c r="M40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>44804</v>
       </c>
@@ -2522,11 +2574,11 @@
       <c r="K41">
         <v>27.2</v>
       </c>
-      <c r="M41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>44804</v>
       </c>
@@ -2561,11 +2613,11 @@
       <c r="K42">
         <v>27.2</v>
       </c>
-      <c r="M42" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>44804</v>
       </c>
@@ -2600,11 +2652,11 @@
       <c r="K43">
         <v>27.2</v>
       </c>
-      <c r="M43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>44804</v>
       </c>
@@ -2639,11 +2691,11 @@
       <c r="K44">
         <v>27.2</v>
       </c>
-      <c r="M44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44804</v>
       </c>
@@ -2678,11 +2730,11 @@
       <c r="K45">
         <v>27.2</v>
       </c>
-      <c r="M45" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44791</v>
       </c>
@@ -2717,11 +2769,11 @@
       <c r="K46">
         <v>29.5</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>44791</v>
       </c>
@@ -2756,11 +2808,11 @@
       <c r="K47">
         <v>29.5</v>
       </c>
-      <c r="M47" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44791</v>
       </c>
@@ -2795,11 +2847,11 @@
       <c r="K48">
         <v>29.5</v>
       </c>
-      <c r="M48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44791</v>
       </c>
@@ -2834,11 +2886,11 @@
       <c r="K49">
         <v>29.5</v>
       </c>
-      <c r="M49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N49" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>44791</v>
       </c>
@@ -2873,11 +2925,11 @@
       <c r="K50">
         <v>29.5</v>
       </c>
-      <c r="M50" t="s">
+      <c r="N50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44791</v>
       </c>
@@ -2912,11 +2964,11 @@
       <c r="K51">
         <v>29.5</v>
       </c>
-      <c r="M51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N51" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>44791</v>
       </c>
@@ -2951,11 +3003,11 @@
       <c r="K52">
         <v>29.5</v>
       </c>
-      <c r="M52" t="s">
+      <c r="N52" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>44791</v>
       </c>
@@ -2990,11 +3042,11 @@
       <c r="K53">
         <v>29.5</v>
       </c>
-      <c r="M53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>44791</v>
       </c>
@@ -3029,11 +3081,11 @@
       <c r="K54">
         <v>29.5</v>
       </c>
-      <c r="M54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>44791</v>
       </c>
@@ -3068,11 +3120,11 @@
       <c r="K55">
         <v>29.5</v>
       </c>
-      <c r="M55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N55" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>44788</v>
       </c>
@@ -3107,11 +3159,11 @@
       <c r="K56">
         <v>28.8</v>
       </c>
-      <c r="M56" t="s">
+      <c r="N56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>44788</v>
       </c>
@@ -3146,11 +3198,11 @@
       <c r="K57">
         <v>28.8</v>
       </c>
-      <c r="M57" t="s">
+      <c r="N57" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>44788</v>
       </c>
@@ -3185,11 +3237,11 @@
       <c r="K58">
         <v>28.8</v>
       </c>
-      <c r="M58" t="s">
+      <c r="N58" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>44788</v>
       </c>
@@ -3224,11 +3276,11 @@
       <c r="K59">
         <v>28.8</v>
       </c>
-      <c r="M59" t="s">
+      <c r="N59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>44788</v>
       </c>
@@ -3263,11 +3315,11 @@
       <c r="K60">
         <v>28.8</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>44822</v>
       </c>
@@ -3302,11 +3354,11 @@
       <c r="K61">
         <v>20.100000000000001</v>
       </c>
-      <c r="M61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>44822</v>
       </c>
@@ -3341,11 +3393,11 @@
       <c r="K62">
         <v>20.100000000000001</v>
       </c>
-      <c r="M62" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N62" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>44822</v>
       </c>
@@ -3380,11 +3432,11 @@
       <c r="K63">
         <v>20.100000000000001</v>
       </c>
-      <c r="M63" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N63" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>44822</v>
       </c>
@@ -3419,11 +3471,11 @@
       <c r="K64">
         <v>20.100000000000001</v>
       </c>
-      <c r="M64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N64" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>44822</v>
       </c>
@@ -3458,11 +3510,11 @@
       <c r="K65">
         <v>20.100000000000001</v>
       </c>
-      <c r="M65" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>44826</v>
       </c>
@@ -3497,11 +3549,11 @@
       <c r="K66">
         <v>28.332999999999998</v>
       </c>
-      <c r="M66" t="s">
+      <c r="N66" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>44826</v>
       </c>
@@ -3536,11 +3588,11 @@
       <c r="K67">
         <v>28.332999999999998</v>
       </c>
-      <c r="M67" t="s">
+      <c r="N67" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>44826</v>
       </c>
@@ -3575,11 +3627,11 @@
       <c r="K68">
         <v>28.332999999999998</v>
       </c>
-      <c r="M68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>44826</v>
       </c>
@@ -3614,11 +3666,11 @@
       <c r="K69">
         <v>28.332999999999998</v>
       </c>
-      <c r="M69" t="s">
+      <c r="N69" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>44826</v>
       </c>
@@ -3653,11 +3705,11 @@
       <c r="K70">
         <v>28.332999999999998</v>
       </c>
-      <c r="M70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N70" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>44826</v>
       </c>
@@ -3692,11 +3744,11 @@
       <c r="K71">
         <v>26.111000000000001</v>
       </c>
-      <c r="M71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N71" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>44826</v>
       </c>
@@ -3731,11 +3783,11 @@
       <c r="K72">
         <v>26.111000000000001</v>
       </c>
-      <c r="M72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N72" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>44826</v>
       </c>
@@ -3770,11 +3822,11 @@
       <c r="K73">
         <v>26.111000000000001</v>
       </c>
-      <c r="M73" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N73" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>44826</v>
       </c>
@@ -3809,11 +3861,11 @@
       <c r="K74">
         <v>26.111000000000001</v>
       </c>
-      <c r="M74" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N74" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>44826</v>
       </c>
@@ -3848,11 +3900,11 @@
       <c r="K75">
         <v>26.111000000000001</v>
       </c>
-      <c r="M75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N75" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>44823</v>
       </c>
@@ -3887,11 +3939,11 @@
       <c r="K76">
         <v>28.332999999999998</v>
       </c>
-      <c r="M76" t="s">
+      <c r="N76" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>44823</v>
       </c>
@@ -3926,11 +3978,11 @@
       <c r="K77">
         <v>28.332999999999998</v>
       </c>
-      <c r="M77" t="s">
+      <c r="N77" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>44823</v>
       </c>
@@ -3965,11 +4017,11 @@
       <c r="K78">
         <v>28.332999999999998</v>
       </c>
-      <c r="M78" t="s">
+      <c r="N78" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>44823</v>
       </c>
@@ -4004,11 +4056,11 @@
       <c r="K79">
         <v>28.332999999999998</v>
       </c>
-      <c r="M79" t="s">
+      <c r="N79" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>44823</v>
       </c>
@@ -4043,11 +4095,11 @@
       <c r="K80">
         <v>28.332999999999998</v>
       </c>
-      <c r="M80" t="s">
+      <c r="N80" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>44861</v>
       </c>
@@ -4082,11 +4134,11 @@
       <c r="K81">
         <v>15</v>
       </c>
-      <c r="M81" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>44861</v>
       </c>
@@ -4121,11 +4173,11 @@
       <c r="K82">
         <v>15</v>
       </c>
-      <c r="M82" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N82" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44861</v>
       </c>
@@ -4160,11 +4212,11 @@
       <c r="K83">
         <v>15</v>
       </c>
-      <c r="M83" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>44861</v>
       </c>
@@ -4199,11 +4251,11 @@
       <c r="K84">
         <v>15</v>
       </c>
-      <c r="M84" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N84" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>44861</v>
       </c>
@@ -4238,11 +4290,11 @@
       <c r="K85">
         <v>15</v>
       </c>
-      <c r="M85" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N85" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>44848</v>
       </c>
@@ -4277,11 +4329,11 @@
       <c r="K86">
         <v>16.666699999999999</v>
       </c>
-      <c r="M86" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N86" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>44848</v>
       </c>
@@ -4316,11 +4368,11 @@
       <c r="K87">
         <v>16.666699999999999</v>
       </c>
-      <c r="M87" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N87" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>44848</v>
       </c>
@@ -4355,11 +4407,11 @@
       <c r="K88">
         <v>16.666699999999999</v>
       </c>
-      <c r="M88" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N88" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>44848</v>
       </c>
@@ -4394,11 +4446,11 @@
       <c r="K89">
         <v>16.666699999999999</v>
       </c>
-      <c r="M89" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N89" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>44848</v>
       </c>
@@ -4433,11 +4485,11 @@
       <c r="K90">
         <v>16.666699999999999</v>
       </c>
-      <c r="M90" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N90" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>44848</v>
       </c>
@@ -4472,11 +4524,11 @@
       <c r="K91">
         <v>16.666699999999999</v>
       </c>
-      <c r="M91" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>44848</v>
       </c>
@@ -4511,11 +4563,11 @@
       <c r="K92">
         <v>16.666699999999999</v>
       </c>
-      <c r="M92" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>44848</v>
       </c>
@@ -4550,11 +4602,11 @@
       <c r="K93">
         <v>16.666699999999999</v>
       </c>
-      <c r="M93" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N93" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>44848</v>
       </c>
@@ -4589,11 +4641,11 @@
       <c r="K94">
         <v>16.666699999999999</v>
       </c>
-      <c r="M94" t="s">
+      <c r="N94" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>44848</v>
       </c>
@@ -4628,11 +4680,11 @@
       <c r="K95">
         <v>16.666699999999999</v>
       </c>
-      <c r="M95" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N95" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>44845</v>
       </c>
@@ -4667,11 +4719,11 @@
       <c r="K96">
         <v>17.777799999999999</v>
       </c>
-      <c r="M96" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N96" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>44845</v>
       </c>
@@ -4706,11 +4758,11 @@
       <c r="K97">
         <v>17.777799999999999</v>
       </c>
-      <c r="M97" t="s">
+      <c r="N97" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>44845</v>
       </c>
@@ -4745,11 +4797,11 @@
       <c r="K98">
         <v>17.777799999999999</v>
       </c>
-      <c r="M98" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N98" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>44845</v>
       </c>
@@ -4784,11 +4836,11 @@
       <c r="K99">
         <v>17.777799999999999</v>
       </c>
-      <c r="M99" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N99" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>44845</v>
       </c>
@@ -4823,11 +4875,11 @@
       <c r="K100">
         <v>17.777799999999999</v>
       </c>
-      <c r="M100" t="s">
+      <c r="N100" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>44878</v>
       </c>
@@ -4862,11 +4914,11 @@
       <c r="K101">
         <v>11.1111</v>
       </c>
-      <c r="M101" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N101" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>44878</v>
       </c>
@@ -4901,11 +4953,11 @@
       <c r="K102">
         <v>11.1111</v>
       </c>
-      <c r="M102" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N102" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>44878</v>
       </c>
@@ -4940,11 +4992,11 @@
       <c r="K103">
         <v>11.1111</v>
       </c>
-      <c r="M103" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N103" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>44878</v>
       </c>
@@ -4979,11 +5031,11 @@
       <c r="K104">
         <v>11.1111</v>
       </c>
-      <c r="M104" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N104" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>44878</v>
       </c>
@@ -5018,11 +5070,11 @@
       <c r="K105">
         <v>11.1111</v>
       </c>
-      <c r="M105" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N105" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>44880</v>
       </c>
@@ -5057,11 +5109,11 @@
       <c r="K106">
         <v>6.6666699999999999</v>
       </c>
-      <c r="M106" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>44880</v>
       </c>
@@ -5096,11 +5148,11 @@
       <c r="K107">
         <v>6.6666699999999999</v>
       </c>
-      <c r="M107" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N107" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>44880</v>
       </c>
@@ -5135,11 +5187,11 @@
       <c r="K108">
         <v>6.6666699999999999</v>
       </c>
-      <c r="M108" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N108" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>44880</v>
       </c>
@@ -5174,11 +5226,11 @@
       <c r="K109">
         <v>6.6666699999999999</v>
       </c>
-      <c r="M109" t="s">
+      <c r="N109" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>44880</v>
       </c>
@@ -5213,11 +5265,11 @@
       <c r="K110">
         <v>6.6666699999999999</v>
       </c>
-      <c r="M110" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N110" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>44882</v>
       </c>
@@ -5252,11 +5304,11 @@
       <c r="K111">
         <v>8.88889</v>
       </c>
-      <c r="M111" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N111" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>44882</v>
       </c>
@@ -5291,11 +5343,11 @@
       <c r="K112">
         <v>8.88889</v>
       </c>
-      <c r="M112" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N112" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>44882</v>
       </c>
@@ -5330,11 +5382,11 @@
       <c r="K113">
         <v>8.88889</v>
       </c>
-      <c r="M113" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N113" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>44882</v>
       </c>
@@ -5369,11 +5421,11 @@
       <c r="K114">
         <v>8.88889</v>
       </c>
-      <c r="M114" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N114" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>44882</v>
       </c>
@@ -5408,11 +5460,11 @@
       <c r="K115">
         <v>8.88889</v>
       </c>
-      <c r="M115" t="s">
+      <c r="N115" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>44882</v>
       </c>
@@ -5447,11 +5499,11 @@
       <c r="K116">
         <v>7.7777799999999999</v>
       </c>
-      <c r="M116" t="s">
+      <c r="N116" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>44882</v>
       </c>
@@ -5486,11 +5538,11 @@
       <c r="K117">
         <v>7.7777799999999999</v>
       </c>
-      <c r="M117" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N117" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>44882</v>
       </c>
@@ -5525,11 +5577,11 @@
       <c r="K118">
         <v>7.7777799999999999</v>
       </c>
-      <c r="M118" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N118" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>44882</v>
       </c>
@@ -5564,11 +5616,11 @@
       <c r="K119">
         <v>7.7777799999999999</v>
       </c>
-      <c r="M119" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N119" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>44882</v>
       </c>
@@ -5603,7 +5655,7 @@
       <c r="K120">
         <v>7.7777799999999999</v>
       </c>
-      <c r="M120" t="s">
+      <c r="N120" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>